<commit_message>
match up works that can be matched up
</commit_message>
<xml_diff>
--- a/combined notes on spreadsheet.xlsx
+++ b/combined notes on spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdewey/Development/code/84000-data-rdf/xml-parsing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEF1373-18D4-094F-9016-812F6810EFF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4366AC56-EB32-2945-9BFE-7DEE75BE9472}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="640" windowWidth="20840" windowHeight="15820" activeTab="3" xr2:uid="{AA1A54E2-02A9-434E-B49F-C824DE424E33}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28540" windowHeight="15760" activeTab="1" xr2:uid="{AA1A54E2-02A9-434E-B49F-C824DE424E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Discrepant roles" sheetId="4" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="946">
   <si>
     <t>84000 ID</t>
   </si>
@@ -2896,16 +2896,56 @@
   </si>
   <si>
     <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+  </si>
+  <si>
+    <t>84000 IDs</t>
+  </si>
+  <si>
+    <t>eft:jinamitra-k-, eft:dzi-na-mi-tra-k-, eft:jinamitra</t>
+  </si>
+  <si>
+    <t>P8217 or P4255</t>
+  </si>
+  <si>
+    <t>eft:klu-i-rgyal-mtshan, eft:cog-ro-klu-i-rgyal-mtshan</t>
+  </si>
+  <si>
+    <t>eft:ban-de-dpal-gyi-lhun-po, eft:dpal-gyi-lhun-po, eft:palgyi-lh-npo</t>
+  </si>
+  <si>
+    <t>eft:ban-de-dpal-brtsegs, eft:ska-ba-dpal-brtsegs, eft:kawa-paltsek-under-the-name-paltsek-raksita-, eft:paltsek</t>
+  </si>
+  <si>
+    <t>P2584</t>
+  </si>
+  <si>
+    <t>eft:prajnavarman, eft:prajnavarma</t>
+  </si>
+  <si>
+    <t>eft:munivarman, eft:munivarma</t>
+  </si>
+  <si>
+    <t>eft:silendrabodhi, eft:surendrabodhi, eft:srilendrabodhi</t>
+  </si>
+  <si>
+    <t>eft:yesh-d-, eft:ye-shes-sde, eft:band-yesh-de, eft:zhang-yesh-d-, eft:yesh-d-ye-shes-sde-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2943,7 +2983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2952,6 +2992,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3284,8 +3325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC99D1F8-999F-3945-A50E-6CC984F32136}">
   <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7195,8 +7236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34985B16-C92D-6243-8507-F700C41B3F78}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7718,8 +7759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9628BDC7-3621-5F4A-829E-B54540E4F224}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD42"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8451,8 +8492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB8AC6A-C797-F64E-A13A-B195FE9524EC}">
   <dimension ref="B1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8492,9 +8533,6 @@
         <v>201</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -8543,9 +8581,6 @@
         <v>6</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -8577,9 +8612,6 @@
         <v>149</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="G7" s="6" t="s">
         <v>932</v>
       </c>
     </row>
@@ -8781,9 +8813,6 @@
         <v>223</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G19" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -8849,6 +8878,9 @@
         <v>229</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>903</v>
       </c>
       <c r="G23" s="4" t="s">
@@ -14137,12 +14169,87 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366B851C-DFC4-054E-B3B8-C10D47165789}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>941</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>945</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>